<commit_message>
no real changes made. Document was used as part of check process for adding collaborators and region/office information to federal agencies. Any alterations to the document were used to help get that information (ie freezing rows to increase readablity)
</commit_message>
<xml_diff>
--- a/documents/Detailed_methods.xlsx
+++ b/documents/Detailed_methods.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/usr/local/bin/store/partner_rff/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/usr/local/bin/store/partner_rff/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703B31EA-D5CB-C042-96ED-3935DD0B4990}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7AD907-9871-C249-9FE1-416E0D8905F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="2360" windowWidth="24640" windowHeight="13740" xr2:uid="{804B5181-2E36-0144-BC00-F5005385D24D}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="24640" windowHeight="13740" xr2:uid="{804B5181-2E36-0144-BC00-F5005385D24D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1752,9 +1752,6 @@
     <t>Central Utah Navajo Sandstone Endemics Conservation Agreement for Aliciella cespitosa (Rabbit Valley gilia or Wonderland alice-flower) Aliciella tenuis (Mussentuchit gilia) Astragalus harrisonii (Harrison’s milkvetch) Cymopterus beckii (Pinnate spring-parsley) Erigeron maguirei (Maguire’s daisy)</t>
   </si>
   <si>
-    <t>USFS Fishlake National Forest, BLM Utah State Office, NPS Capitol Reef National Park, USFWS Utah Field Office</t>
-  </si>
-  <si>
     <t>While other species are present in agreement, all partners of the agreement were partnered for this particular species</t>
   </si>
   <si>
@@ -2383,6 +2380,9 @@
   </si>
   <si>
     <t>I don't think this is a partnership</t>
+  </si>
+  <si>
+    <t>USFS Fishlake National Forest, BLM Utah State Office, BLM Richfield Field Office, BLM Price Field Office, NPS Capitol Reef National Park, USFWS Utah Field Office</t>
   </si>
 </sst>
 </file>
@@ -2438,7 +2438,7 @@
       <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2493,6 +2493,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2507,7 +2513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -2544,6 +2550,12 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2866,16 +2878,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77EAF11B-F2D7-D245-AF69-27A36AF6775A}">
   <dimension ref="A1:XDX142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H125" sqref="H125"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="10" max="10" width="3.1640625" customWidth="1"/>
     <col min="12" max="12" width="21.5" style="9" customWidth="1"/>
-    <col min="13" max="24" width="10.83203125" style="9"/>
+    <col min="13" max="17" width="10.83203125" style="9"/>
+    <col min="18" max="18" width="10.83203125" style="17"/>
+    <col min="19" max="19" width="10.83203125" style="5"/>
+    <col min="20" max="24" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16352">
@@ -2892,25 +2907,25 @@
         <v>311</v>
       </c>
       <c r="E1" t="s">
+        <v>603</v>
+      </c>
+      <c r="F1" t="s">
         <v>604</v>
-      </c>
-      <c r="F1" t="s">
-        <v>605</v>
       </c>
       <c r="G1" t="s">
         <v>186</v>
       </c>
       <c r="H1" t="s">
+        <v>601</v>
+      </c>
+      <c r="I1" t="s">
         <v>602</v>
-      </c>
-      <c r="I1" t="s">
-        <v>603</v>
       </c>
       <c r="J1" t="s">
         <v>177</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>178</v>
@@ -2930,10 +2945,10 @@
       <c r="Q1" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="5" t="s">
         <v>181</v>
       </c>
       <c r="T1" s="9" t="s">
@@ -2955,13 +2970,13 @@
         <v>187</v>
       </c>
       <c r="Z1" t="s">
+        <v>712</v>
+      </c>
+      <c r="AA1" t="s">
         <v>713</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>714</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>715</v>
       </c>
       <c r="AC1" t="s">
         <v>302</v>
@@ -2981,7 +2996,7 @@
         <v>312</v>
       </c>
       <c r="F2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G2" t="s">
         <v>198</v>
@@ -3013,10 +3028,10 @@
       <c r="Q2" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R2" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S2" s="11" t="s">
+      <c r="R2" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S2" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T2" s="11" t="s">
@@ -3041,7 +3056,7 @@
         <v>303</v>
       </c>
       <c r="AA2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="AB2" t="s">
         <v>301</v>
@@ -3064,7 +3079,7 @@
         <v>313</v>
       </c>
       <c r="F3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>192</v>
@@ -3099,10 +3114,10 @@
       <c r="Q3" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="S3" s="5" t="s">
         <v>314</v>
       </c>
       <c r="T3" s="9" t="s">
@@ -3127,7 +3142,7 @@
         <v>305</v>
       </c>
       <c r="AA3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="AB3" t="s">
         <v>205</v>
@@ -3144,7 +3159,7 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G4" t="s">
         <v>198</v>
@@ -3179,10 +3194,10 @@
       <c r="Q4" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="R4" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="S4" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T4" s="9" t="s">
@@ -3207,7 +3222,7 @@
         <v>315</v>
       </c>
       <c r="AA4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="AB4" t="s">
         <v>316</v>
@@ -3250,10 +3265,10 @@
       <c r="Q5" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R5" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S5" s="9" t="s">
+      <c r="R5" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S5" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T5" s="9" t="s">
@@ -3281,13 +3296,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D6" t="s">
         <v>321</v>
       </c>
       <c r="F6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>192</v>
@@ -3302,10 +3317,10 @@
         <v>177</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="M6" s="9" t="s">
         <v>194</v>
@@ -3322,10 +3337,10 @@
       <c r="Q6" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="R6" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="S6" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T6" s="9" t="s">
@@ -3350,7 +3365,7 @@
         <v>324</v>
       </c>
       <c r="AA6" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="AB6" t="s">
         <v>325</v>
@@ -3365,7 +3380,7 @@
         <v>177</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J7" t="s">
         <v>177</v>
@@ -3374,7 +3389,7 @@
         <v>316</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="M7" s="9" t="s">
         <v>195</v>
@@ -3391,10 +3406,10 @@
       <c r="Q7" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="R7" s="17" t="s">
         <v>335</v>
       </c>
-      <c r="S7" s="9" t="s">
+      <c r="S7" s="5" t="s">
         <v>336</v>
       </c>
       <c r="T7" s="9" t="s">
@@ -19773,10 +19788,10 @@
       <c r="Q8" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="R8" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S8" s="9" t="s">
+      <c r="R8" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S8" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T8" s="9" t="s">
@@ -36134,7 +36149,7 @@
         <v>177</v>
       </c>
       <c r="F9" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>192</v>
@@ -36169,10 +36184,10 @@
       <c r="Q9" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R9" s="9" t="s">
+      <c r="R9" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S9" s="9" t="s">
+      <c r="S9" s="5" t="s">
         <v>337</v>
       </c>
       <c r="T9" s="9" t="s">
@@ -36197,7 +36212,7 @@
         <v>303</v>
       </c>
       <c r="AA9" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="AB9" t="s">
         <v>205</v>
@@ -36217,7 +36232,7 @@
         <v>342</v>
       </c>
       <c r="F10" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>192</v>
@@ -36252,10 +36267,10 @@
       <c r="Q10" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="R10" s="17" t="s">
         <v>340</v>
       </c>
-      <c r="S10" s="9" t="s">
+      <c r="S10" s="5" t="s">
         <v>341</v>
       </c>
       <c r="T10" s="9" t="s">
@@ -36280,7 +36295,7 @@
         <v>303</v>
       </c>
       <c r="AA10" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="AB10" t="s">
         <v>205</v>
@@ -36303,7 +36318,7 @@
         <v>346</v>
       </c>
       <c r="F11" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G11" t="s">
         <v>198</v>
@@ -36318,7 +36333,7 @@
         <v>177</v>
       </c>
       <c r="K11" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L11" s="9" t="s">
         <v>347</v>
@@ -36338,10 +36353,10 @@
       <c r="Q11" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R11" s="9" t="s">
+      <c r="R11" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S11" s="9" t="s">
+      <c r="S11" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T11" s="9" t="s">
@@ -36386,10 +36401,10 @@
         <v>357</v>
       </c>
       <c r="E12" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="F12" t="s">
         <v>614</v>
-      </c>
-      <c r="F12" t="s">
-        <v>615</v>
       </c>
       <c r="G12" t="s">
         <v>198</v>
@@ -36424,10 +36439,10 @@
       <c r="Q12" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R12" s="9" t="s">
+      <c r="R12" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S12" s="9" t="s">
+      <c r="S12" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T12" s="9" t="s">
@@ -36452,7 +36467,7 @@
         <v>348</v>
       </c>
       <c r="AA12" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="AB12" t="s">
         <v>349</v>
@@ -36486,10 +36501,10 @@
       <c r="Q13" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R13" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S13" s="11" t="s">
+      <c r="R13" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S13" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T13" s="11" t="s">
@@ -36534,10 +36549,10 @@
       <c r="Q14" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R14" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S14" s="11" t="s">
+      <c r="R14" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S14" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T14" s="11" t="s">
@@ -36582,10 +36597,10 @@
       <c r="Q15" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R15" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S15" s="11" t="s">
+      <c r="R15" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S15" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T15" s="11" t="s">
@@ -36630,10 +36645,10 @@
       <c r="Q16" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R16" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S16" s="11" t="s">
+      <c r="R16" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S16" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T16" s="11" t="s">
@@ -36665,7 +36680,7 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>200</v>
@@ -36700,10 +36715,10 @@
       <c r="Q17" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R17" s="11" t="s">
+      <c r="R17" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="S17" s="11" t="s">
+      <c r="S17" s="34" t="s">
         <v>203</v>
       </c>
       <c r="T17" s="11" t="s">
@@ -36728,7 +36743,7 @@
         <v>358</v>
       </c>
       <c r="AA17" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="AB17" t="s">
         <v>316</v>
@@ -36748,7 +36763,7 @@
         <v>177</v>
       </c>
       <c r="F18" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>200</v>
@@ -36783,10 +36798,10 @@
       <c r="Q18" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R18" s="11" t="s">
+      <c r="R18" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="S18" s="9" t="s">
+      <c r="S18" s="5" t="s">
         <v>364</v>
       </c>
       <c r="T18" s="11" t="s">
@@ -36811,7 +36826,7 @@
         <v>361</v>
       </c>
       <c r="AA18" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="AB18" t="s">
         <v>362</v>
@@ -36845,10 +36860,10 @@
       <c r="Q19" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R19" s="11" t="s">
+      <c r="R19" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="S19" s="11" t="s">
+      <c r="S19" s="34" t="s">
         <v>203</v>
       </c>
       <c r="T19" s="11" t="s">
@@ -36879,7 +36894,7 @@
         <v>177</v>
       </c>
       <c r="F20" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>192</v>
@@ -36914,10 +36929,10 @@
       <c r="Q20" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R20" s="11" t="s">
+      <c r="R20" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="S20" s="11" t="s">
+      <c r="S20" s="34" t="s">
         <v>371</v>
       </c>
       <c r="T20" s="11" t="s">
@@ -36942,7 +36957,7 @@
         <v>367</v>
       </c>
       <c r="AA20" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="AB20" t="s">
         <v>368</v>
@@ -36965,7 +36980,7 @@
         <v>346</v>
       </c>
       <c r="F21" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>192</v>
@@ -37000,10 +37015,10 @@
       <c r="Q21" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R21" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S21" s="11" t="s">
+      <c r="R21" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S21" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T21" s="11" t="s">
@@ -37028,7 +37043,7 @@
         <v>372</v>
       </c>
       <c r="AA21" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="AB21" t="s">
         <v>301</v>
@@ -37065,10 +37080,10 @@
       <c r="Q22" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R22" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S22" s="11" t="s">
+      <c r="R22" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S22" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T22" s="11" t="s">
@@ -37099,7 +37114,7 @@
         <v>177</v>
       </c>
       <c r="F23" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>192</v>
@@ -37134,10 +37149,10 @@
       <c r="Q23" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R23" s="11" t="s">
+      <c r="R23" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="S23" s="9" t="s">
+      <c r="S23" s="5" t="s">
         <v>379</v>
       </c>
       <c r="T23" s="11" t="s">
@@ -37162,7 +37177,7 @@
         <v>377</v>
       </c>
       <c r="AA23" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="AB23" t="s">
         <v>378</v>
@@ -37186,7 +37201,7 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>200</v>
@@ -37221,10 +37236,10 @@
       <c r="Q24" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R24" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S24" s="11" t="s">
+      <c r="R24" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S24" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T24" s="11" t="s">
@@ -37249,7 +37264,7 @@
         <v>381</v>
       </c>
       <c r="AA24" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="AB24" t="s">
         <v>373</v>
@@ -37293,10 +37308,10 @@
       <c r="Q25" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R25" s="11" t="s">
+      <c r="R25" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="S25" s="11" t="s">
+      <c r="S25" s="34" t="s">
         <v>203</v>
       </c>
       <c r="T25" s="11" t="s">
@@ -37332,10 +37347,10 @@
         <v>177</v>
       </c>
       <c r="E26" s="24" t="s">
+        <v>621</v>
+      </c>
+      <c r="F26" t="s">
         <v>622</v>
-      </c>
-      <c r="F26" t="s">
-        <v>623</v>
       </c>
       <c r="G26" t="e">
         <v>#N/A</v>
@@ -37367,10 +37382,10 @@
       <c r="Q26" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="R26" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S26" s="9" t="s">
+      <c r="R26" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S26" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T26" s="9" t="s">
@@ -37395,7 +37410,7 @@
         <v>348</v>
       </c>
       <c r="AA26" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB26" t="s">
         <v>301</v>
@@ -37415,7 +37430,7 @@
         <v>177</v>
       </c>
       <c r="F27" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="G27" t="e">
         <v>#N/A</v>
@@ -37447,10 +37462,10 @@
       <c r="Q27" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="R27" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S27" s="9" t="s">
+      <c r="R27" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S27" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T27" s="9" t="s">
@@ -37475,7 +37490,7 @@
         <v>348</v>
       </c>
       <c r="AA27" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB27" t="s">
         <v>301</v>
@@ -37495,7 +37510,7 @@
         <v>177</v>
       </c>
       <c r="F28" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G28" t="e">
         <v>#N/A</v>
@@ -37527,10 +37542,10 @@
       <c r="Q28" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="R28" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S28" s="9" t="s">
+      <c r="R28" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S28" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T28" s="9" t="s">
@@ -37555,7 +37570,7 @@
         <v>348</v>
       </c>
       <c r="AA28" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB28" t="s">
         <v>301</v>
@@ -37575,7 +37590,7 @@
         <v>177</v>
       </c>
       <c r="F29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="G29" t="s">
         <v>198</v>
@@ -37607,10 +37622,10 @@
       <c r="Q29" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="R29" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S29" s="9" t="s">
+      <c r="R29" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S29" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T29" s="9" t="s">
@@ -37635,7 +37650,7 @@
         <v>348</v>
       </c>
       <c r="AA29" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB29" t="s">
         <v>301</v>
@@ -37655,7 +37670,7 @@
         <v>390</v>
       </c>
       <c r="F30" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>192</v>
@@ -37670,7 +37685,7 @@
         <v>177</v>
       </c>
       <c r="K30" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="L30" s="9" t="s">
         <v>388</v>
@@ -37690,10 +37705,10 @@
       <c r="Q30" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R30" s="9" t="s">
+      <c r="R30" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S30" s="9" t="s">
+      <c r="S30" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T30" s="9" t="s">
@@ -37718,10 +37733,10 @@
         <v>385</v>
       </c>
       <c r="AA30" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="AB30" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="AC30">
         <v>10</v>
@@ -37752,10 +37767,10 @@
       <c r="Q31" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R31" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S31" s="9" t="s">
+      <c r="R31" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S31" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T31" s="9" t="s">
@@ -37787,7 +37802,7 @@
         <v>177</v>
       </c>
       <c r="F32" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G32" s="24" t="s">
         <v>200</v>
@@ -37819,10 +37834,10 @@
       <c r="Q32" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R32" s="9" t="s">
+      <c r="R32" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S32" s="9" t="s">
+      <c r="S32" s="5" t="s">
         <v>393</v>
       </c>
       <c r="T32" s="9" t="s">
@@ -37847,7 +37862,7 @@
         <v>367</v>
       </c>
       <c r="AA32" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="AB32" t="s">
         <v>391</v>
@@ -37870,7 +37885,7 @@
         <v>177</v>
       </c>
       <c r="F33" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G33" s="17" t="s">
         <v>192</v>
@@ -37902,10 +37917,10 @@
       <c r="Q33" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R33" s="9" t="s">
+      <c r="R33" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S33" s="9" t="s">
+      <c r="S33" s="5" t="s">
         <v>209</v>
       </c>
       <c r="T33" s="9" t="s">
@@ -37930,10 +37945,10 @@
         <v>394</v>
       </c>
       <c r="AA33" t="s">
+        <v>729</v>
+      </c>
+      <c r="AB33" t="s">
         <v>730</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>731</v>
       </c>
       <c r="AC33">
         <v>6</v>
@@ -37951,7 +37966,7 @@
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>192</v>
@@ -37984,10 +37999,10 @@
       <c r="Q34" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R34" s="9" t="s">
+      <c r="R34" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S34" s="9" t="s">
+      <c r="S34" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T34" s="9" t="s">
@@ -38012,7 +38027,7 @@
         <v>305</v>
       </c>
       <c r="AA34" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AB34" t="s">
         <v>396</v>
@@ -38035,7 +38050,7 @@
         <v>200</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>198</v>
@@ -38065,10 +38080,10 @@
       <c r="Q35" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R35" s="12" t="s">
+      <c r="R35" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="S35" s="12" t="s">
+      <c r="S35" s="35" t="s">
         <v>213</v>
       </c>
       <c r="T35" s="12" t="s">
@@ -38090,10 +38105,10 @@
         <v>1996</v>
       </c>
       <c r="Z35" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="AA35" s="2" t="s">
         <v>733</v>
-      </c>
-      <c r="AA35" s="2" t="s">
-        <v>734</v>
       </c>
       <c r="AB35" s="2" t="s">
         <v>301</v>
@@ -38132,10 +38147,10 @@
       <c r="Q36" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R36" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="S36" s="12" t="s">
+      <c r="R36" s="38" t="s">
+        <v>301</v>
+      </c>
+      <c r="S36" s="35" t="s">
         <v>301</v>
       </c>
       <c r="T36" s="12" t="s">
@@ -38168,10 +38183,10 @@
         <v>47</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F37" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G37" s="7" t="s">
         <v>192</v>
@@ -38186,7 +38201,7 @@
         <v>177</v>
       </c>
       <c r="K37" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L37" s="9" t="s">
         <v>407</v>
@@ -38206,10 +38221,10 @@
       <c r="Q37" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R37" s="9" t="s">
+      <c r="R37" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="S37" s="9" t="s">
+      <c r="S37" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T37" s="12" t="s">
@@ -38234,10 +38249,10 @@
         <v>402</v>
       </c>
       <c r="AA37" t="s">
+        <v>734</v>
+      </c>
+      <c r="AB37" t="s">
         <v>735</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>736</v>
       </c>
       <c r="AC37">
         <v>17</v>
@@ -38251,7 +38266,7 @@
         <v>177</v>
       </c>
       <c r="K38" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L38" s="9" t="s">
         <v>408</v>
@@ -38271,10 +38286,10 @@
       <c r="Q38" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R38" s="9" t="s">
+      <c r="R38" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="S38" s="9" t="s">
+      <c r="S38" s="5" t="s">
         <v>217</v>
       </c>
       <c r="T38" s="12" t="s">
@@ -38305,10 +38320,10 @@
         <v>177</v>
       </c>
       <c r="F39" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G39" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="H39" t="e">
         <v>#N/A</v>
@@ -38340,10 +38355,10 @@
       <c r="Q39" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R39" s="9" t="s">
+      <c r="R39" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S39" s="9" t="s">
+      <c r="S39" s="5" t="s">
         <v>220</v>
       </c>
       <c r="T39" s="12" t="s">
@@ -38368,7 +38383,7 @@
         <v>404</v>
       </c>
       <c r="AA39" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="AB39" t="s">
         <v>405</v>
@@ -38388,7 +38403,7 @@
         <v>177</v>
       </c>
       <c r="F40" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G40" t="e">
         <v>#N/A</v>
@@ -38423,10 +38438,10 @@
       <c r="Q40" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R40" s="9" t="s">
+      <c r="R40" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S40" s="9" t="s">
+      <c r="S40" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T40" s="9" t="s">
@@ -38451,7 +38466,7 @@
         <v>358</v>
       </c>
       <c r="AA40" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="AB40" t="s">
         <v>406</v>
@@ -38475,7 +38490,7 @@
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>200</v>
@@ -38490,7 +38505,7 @@
         <v>177</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L41" s="9" t="s">
         <v>411</v>
@@ -38510,10 +38525,10 @@
       <c r="Q41" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R41" s="9" t="s">
+      <c r="R41" s="17" t="s">
         <v>414</v>
       </c>
-      <c r="S41" s="9" t="s">
+      <c r="S41" s="5" t="s">
         <v>227</v>
       </c>
       <c r="T41" s="9" t="s">
@@ -38538,10 +38553,10 @@
         <v>413</v>
       </c>
       <c r="AA41" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="AB41" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="AC41">
         <v>11</v>
@@ -38580,10 +38595,10 @@
       <c r="Q42" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R42" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S42" s="9" t="s">
+      <c r="R42" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S42" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T42" s="9" t="s">
@@ -38614,7 +38629,7 @@
         <v>177</v>
       </c>
       <c r="F43" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G43" t="s">
         <v>198</v>
@@ -38646,10 +38661,10 @@
       <c r="Q43" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R43" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S43" s="9" t="s">
+      <c r="R43" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S43" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T43" s="9" t="s">
@@ -38671,10 +38686,10 @@
         <v>1998</v>
       </c>
       <c r="Z43" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="AA43" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB43" t="s">
         <v>301</v>
@@ -38694,7 +38709,7 @@
         <v>177</v>
       </c>
       <c r="F44" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G44" t="s">
         <v>198</v>
@@ -38726,10 +38741,10 @@
       <c r="Q44" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R44" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S44" s="9" t="s">
+      <c r="R44" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S44" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T44" s="9" t="s">
@@ -38754,7 +38769,7 @@
         <v>348</v>
       </c>
       <c r="AA44" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB44" t="s">
         <v>301</v>
@@ -38771,13 +38786,13 @@
         <v>59</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F45" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="G45" t="s">
         <v>198</v>
@@ -38809,10 +38824,10 @@
       <c r="Q45" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R45" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S45" s="11" t="s">
+      <c r="R45" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S45" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T45" s="11" t="s">
@@ -38837,7 +38852,7 @@
         <v>418</v>
       </c>
       <c r="AA45" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="AB45" t="s">
         <v>301</v>
@@ -38857,7 +38872,7 @@
         <v>177</v>
       </c>
       <c r="F46" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>192</v>
@@ -38892,10 +38907,10 @@
       <c r="Q46" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R46" s="9" t="s">
+      <c r="R46" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="S46" s="9" t="s">
+      <c r="S46" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T46" s="9" t="s">
@@ -38920,7 +38935,7 @@
         <v>423</v>
       </c>
       <c r="AA46" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="AB46" t="s">
         <v>424</v>
@@ -38943,7 +38958,7 @@
         <v>177</v>
       </c>
       <c r="F47" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G47" t="s">
         <v>198</v>
@@ -38978,10 +38993,10 @@
       <c r="Q47" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R47" t="s">
+      <c r="R47" s="17" t="s">
         <v>428</v>
       </c>
-      <c r="S47" s="9" t="s">
+      <c r="S47" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T47" s="9" t="s">
@@ -39006,7 +39021,7 @@
         <v>303</v>
       </c>
       <c r="AA47" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="AB47" t="s">
         <v>427</v>
@@ -39026,7 +39041,7 @@
         <v>177</v>
       </c>
       <c r="F48" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G48" t="s">
         <v>198</v>
@@ -39061,10 +39076,10 @@
       <c r="Q48" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R48" s="9" t="s">
+      <c r="R48" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S48" s="9" t="s">
+      <c r="S48" s="5" t="s">
         <v>237</v>
       </c>
       <c r="T48" s="9" t="s">
@@ -39089,7 +39104,7 @@
         <v>430</v>
       </c>
       <c r="AA48" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="AB48" t="s">
         <v>431</v>
@@ -39112,13 +39127,13 @@
         <v>438</v>
       </c>
       <c r="F49" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>192</v>
       </c>
       <c r="H49" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I49" t="e">
         <v>#N/A</v>
@@ -39147,10 +39162,10 @@
       <c r="Q49" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R49" t="s">
+      <c r="R49" s="17" t="s">
         <v>437</v>
       </c>
-      <c r="S49" s="9" t="s">
+      <c r="S49" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T49" s="9" t="s">
@@ -39175,7 +39190,7 @@
         <v>303</v>
       </c>
       <c r="AA49" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="AB49" t="s">
         <v>253</v>
@@ -39195,7 +39210,7 @@
         <v>177</v>
       </c>
       <c r="F50" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G50" s="24" t="s">
         <v>200</v>
@@ -39204,7 +39219,7 @@
         <v>192</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="J50" t="s">
         <v>177</v>
@@ -39228,10 +39243,10 @@
       <c r="Q50" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R50" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S50" s="9" t="s">
+      <c r="R50" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S50" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T50" s="9" t="s">
@@ -39256,7 +39271,7 @@
         <v>348</v>
       </c>
       <c r="AA50" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB50" t="s">
         <v>301</v>
@@ -39276,16 +39291,16 @@
         <v>177</v>
       </c>
       <c r="E51" s="24" t="s">
+        <v>644</v>
+      </c>
+      <c r="F51" t="s">
         <v>645</v>
-      </c>
-      <c r="F51" t="s">
-        <v>646</v>
       </c>
       <c r="G51" s="24" t="s">
         <v>192</v>
       </c>
       <c r="H51" s="24" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I51" s="24" t="s">
         <v>200</v>
@@ -39312,10 +39327,10 @@
       <c r="Q51" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R51" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S51" s="9" t="s">
+      <c r="R51" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S51" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T51" s="9" t="s">
@@ -39340,7 +39355,7 @@
         <v>348</v>
       </c>
       <c r="AA51" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB51" t="s">
         <v>301</v>
@@ -39360,16 +39375,16 @@
         <v>177</v>
       </c>
       <c r="E52" s="24" t="s">
+        <v>644</v>
+      </c>
+      <c r="F52" t="s">
         <v>645</v>
-      </c>
-      <c r="F52" t="s">
-        <v>646</v>
       </c>
       <c r="G52" s="24" t="s">
         <v>192</v>
       </c>
       <c r="H52" s="24" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I52" s="24" t="s">
         <v>200</v>
@@ -39396,10 +39411,10 @@
       <c r="Q52" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R52" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S52" s="9" t="s">
+      <c r="R52" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S52" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T52" s="9" t="s">
@@ -39424,7 +39439,7 @@
         <v>348</v>
       </c>
       <c r="AA52" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB52" t="s">
         <v>301</v>
@@ -39444,7 +39459,7 @@
         <v>177</v>
       </c>
       <c r="F53" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G53" s="7" t="s">
         <v>192</v>
@@ -39479,10 +39494,10 @@
       <c r="Q53" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R53" s="9" t="s">
+      <c r="R53" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="S53" s="9" t="s">
+      <c r="S53" s="5" t="s">
         <v>436</v>
       </c>
       <c r="T53" s="9" t="s">
@@ -39507,7 +39522,7 @@
         <v>439</v>
       </c>
       <c r="AA53" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="AB53" t="s">
         <v>205</v>
@@ -39529,7 +39544,7 @@
       <c r="D54" s="9"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>198</v>
@@ -39548,7 +39563,7 @@
         <v>177</v>
       </c>
       <c r="M54" s="10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="N54" s="9" t="s">
         <v>387</v>
@@ -39562,10 +39577,10 @@
       <c r="Q54" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R54" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S54" s="9" t="s">
+      <c r="R54" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S54" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T54" s="9" t="s">
@@ -39590,7 +39605,7 @@
         <v>348</v>
       </c>
       <c r="AA54" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB54" t="s">
         <v>301</v>
@@ -39611,7 +39626,7 @@
       </c>
       <c r="D55" s="9"/>
       <c r="F55" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G55" t="s">
         <v>198</v>
@@ -39626,7 +39641,7 @@
         <v>177</v>
       </c>
       <c r="M55" s="10" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="N55" s="9" t="s">
         <v>387</v>
@@ -39640,10 +39655,10 @@
       <c r="Q55" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R55" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S55" s="9" t="s">
+      <c r="R55" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S55" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T55" s="9" t="s">
@@ -39668,7 +39683,7 @@
         <v>348</v>
       </c>
       <c r="AA55" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB55" t="s">
         <v>301</v>
@@ -39691,7 +39706,7 @@
         <v>177</v>
       </c>
       <c r="F56" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G56" s="7" t="s">
         <v>192</v>
@@ -39726,10 +39741,10 @@
       <c r="Q56" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R56" s="9" t="s">
+      <c r="R56" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S56" s="9" t="s">
+      <c r="S56" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T56" s="9" t="s">
@@ -39754,7 +39769,7 @@
         <v>404</v>
       </c>
       <c r="AA56" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="AB56" t="s">
         <v>440</v>
@@ -39776,7 +39791,7 @@
       <c r="D57" s="9"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G57" s="2" t="e">
         <v>#N/A</v>
@@ -39798,7 +39813,7 @@
         <v>478</v>
       </c>
       <c r="N57" s="9" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="O57" s="9">
         <v>0</v>
@@ -39809,10 +39824,10 @@
       <c r="Q57" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R57" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S57" s="9" t="s">
+      <c r="R57" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S57" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T57" s="9" t="s">
@@ -39837,7 +39852,7 @@
         <v>348</v>
       </c>
       <c r="AA57" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB57" t="s">
         <v>301</v>
@@ -39857,7 +39872,7 @@
         <v>177</v>
       </c>
       <c r="F58" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G58" s="7" t="s">
         <v>192</v>
@@ -39892,10 +39907,10 @@
       <c r="Q58" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R58" s="9" t="s">
+      <c r="R58" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S58" s="9" t="s">
+      <c r="S58" s="5" t="s">
         <v>446</v>
       </c>
       <c r="T58" s="9" t="s">
@@ -39920,7 +39935,7 @@
         <v>442</v>
       </c>
       <c r="AA58" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AB58" t="s">
         <v>443</v>
@@ -39943,13 +39958,13 @@
         <v>438</v>
       </c>
       <c r="F59" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G59" s="17" t="s">
         <v>192</v>
       </c>
       <c r="H59" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I59" t="e">
         <v>#N/A</v>
@@ -39975,10 +39990,10 @@
       <c r="Q59" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R59" t="s">
+      <c r="R59" s="17" t="s">
         <v>437</v>
       </c>
-      <c r="S59" s="9" t="s">
+      <c r="S59" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T59" s="9" t="s">
@@ -40003,7 +40018,7 @@
         <v>303</v>
       </c>
       <c r="AA59" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="AB59" t="s">
         <v>253</v>
@@ -40024,7 +40039,7 @@
       </c>
       <c r="D60" s="9"/>
       <c r="F60" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G60" t="s">
         <v>198</v>
@@ -40056,10 +40071,10 @@
       <c r="Q60" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R60" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S60" s="9" t="s">
+      <c r="R60" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S60" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T60" s="9" t="s">
@@ -40081,10 +40096,10 @@
         <v>2012</v>
       </c>
       <c r="Z60" t="s">
+        <v>747</v>
+      </c>
+      <c r="AA60" t="s">
         <v>748</v>
-      </c>
-      <c r="AA60" t="s">
-        <v>749</v>
       </c>
       <c r="AB60" t="s">
         <v>301</v>
@@ -40104,7 +40119,7 @@
         <v>177</v>
       </c>
       <c r="F61" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>192</v>
@@ -40139,10 +40154,10 @@
       <c r="Q61" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R61" s="9" t="s">
+      <c r="R61" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S61" s="9" t="s">
+      <c r="S61" s="5" t="s">
         <v>449</v>
       </c>
       <c r="T61" s="9" t="s">
@@ -40167,7 +40182,7 @@
         <v>442</v>
       </c>
       <c r="AA61" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="AB61" t="s">
         <v>447</v>
@@ -40190,7 +40205,7 @@
         <v>177</v>
       </c>
       <c r="F62" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G62" s="24" t="s">
         <v>200</v>
@@ -40225,10 +40240,10 @@
       <c r="Q62" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R62" s="9" t="s">
+      <c r="R62" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S62" s="9" t="s">
+      <c r="S62" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T62" s="9" t="s">
@@ -40253,7 +40268,7 @@
         <v>348</v>
       </c>
       <c r="AA62" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="AB62" t="s">
         <v>450</v>
@@ -40274,7 +40289,7 @@
       </c>
       <c r="D63" s="9"/>
       <c r="F63" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G63" t="s">
         <v>198</v>
@@ -40306,10 +40321,10 @@
       <c r="Q63" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R63" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S63" s="9" t="s">
+      <c r="R63" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S63" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T63" s="9" t="s">
@@ -40334,7 +40349,7 @@
         <v>348</v>
       </c>
       <c r="AA63" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB63" t="s">
         <v>301</v>
@@ -40354,7 +40369,7 @@
         <v>454</v>
       </c>
       <c r="F64" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G64" t="s">
         <v>198</v>
@@ -40389,10 +40404,10 @@
       <c r="Q64" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R64" s="9" t="s">
+      <c r="R64" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="S64" s="9" t="s">
+      <c r="S64" s="5" t="s">
         <v>248</v>
       </c>
       <c r="T64" s="9" t="s">
@@ -40417,7 +40432,7 @@
         <v>404</v>
       </c>
       <c r="AA64" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="AB64" t="s">
         <v>453</v>
@@ -40434,19 +40449,19 @@
         <v>97</v>
       </c>
       <c r="C65" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D65" t="s">
         <v>177</v>
       </c>
       <c r="E65" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="F65" t="s">
         <v>658</v>
       </c>
-      <c r="F65" t="s">
-        <v>659</v>
-      </c>
       <c r="G65" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="H65" t="e">
         <v>#N/A</v>
@@ -40458,7 +40473,7 @@
         <v>177</v>
       </c>
       <c r="K65" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L65" s="9" t="s">
         <v>460</v>
@@ -40478,10 +40493,10 @@
       <c r="Q65" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R65" s="9" t="s">
+      <c r="R65" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S65" s="9" t="s">
+      <c r="S65" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T65" s="9" t="s">
@@ -40506,7 +40521,7 @@
         <v>457</v>
       </c>
       <c r="AA65" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="AB65" t="s">
         <v>458</v>
@@ -40523,7 +40538,7 @@
         <v>177</v>
       </c>
       <c r="K66" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L66" s="9" t="s">
         <v>462</v>
@@ -40543,10 +40558,10 @@
       <c r="Q66" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R66" s="9" t="s">
+      <c r="R66" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="S66" s="9" t="s">
+      <c r="S66" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T66" s="9" t="s">
@@ -40574,7 +40589,7 @@
         <v>177</v>
       </c>
       <c r="K67" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L67" s="9" t="s">
         <v>461</v>
@@ -40594,10 +40609,10 @@
       <c r="Q67" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R67" s="9" t="s">
+      <c r="R67" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="S67" s="18" t="s">
+      <c r="S67" s="36" t="s">
         <v>203</v>
       </c>
       <c r="T67" s="18" t="s">
@@ -40629,7 +40644,7 @@
       </c>
       <c r="D68" s="9"/>
       <c r="F68" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G68" t="s">
         <v>198</v>
@@ -40662,10 +40677,10 @@
       <c r="Q68" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R68" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S68" s="11" t="s">
+      <c r="R68" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S68" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T68" s="11" t="s">
@@ -40690,7 +40705,7 @@
         <v>348</v>
       </c>
       <c r="AA68" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB68" t="s">
         <v>301</v>
@@ -40710,7 +40725,7 @@
         <v>468</v>
       </c>
       <c r="F69" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G69" s="7" t="s">
         <v>200</v>
@@ -40742,10 +40757,10 @@
       <c r="Q69" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R69" s="9" t="s">
+      <c r="R69" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S69" s="9" t="s">
+      <c r="S69" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T69" s="9" t="s">
@@ -40770,10 +40785,10 @@
         <v>463</v>
       </c>
       <c r="AA69" t="s">
+        <v>753</v>
+      </c>
+      <c r="AB69" t="s">
         <v>754</v>
-      </c>
-      <c r="AB69" t="s">
-        <v>755</v>
       </c>
       <c r="AC69">
         <v>6</v>
@@ -40790,7 +40805,7 @@
         <v>177</v>
       </c>
       <c r="K70" s="9" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L70" s="9" t="s">
         <v>467</v>
@@ -40810,10 +40825,10 @@
       <c r="Q70" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R70" s="9" t="s">
+      <c r="R70" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="S70" s="9" t="s">
+      <c r="S70" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T70" s="9" t="s">
@@ -40845,7 +40860,7 @@
       </c>
       <c r="D71" s="9"/>
       <c r="F71" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G71" t="s">
         <v>198</v>
@@ -40866,7 +40881,7 @@
         <v>474</v>
       </c>
       <c r="N71" s="9" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="O71" s="9">
         <v>0</v>
@@ -40877,10 +40892,10 @@
       <c r="Q71" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R71" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S71" s="11" t="s">
+      <c r="R71" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S71" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T71" s="11" t="s">
@@ -40905,7 +40920,7 @@
         <v>348</v>
       </c>
       <c r="AA71" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB71" t="s">
         <v>301</v>
@@ -40925,7 +40940,7 @@
         <v>177</v>
       </c>
       <c r="F72" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G72" t="e">
         <v>#N/A</v>
@@ -40960,10 +40975,10 @@
       <c r="Q72" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R72" s="9" t="s">
+      <c r="R72" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S72" s="9" t="s">
+      <c r="S72" s="5" t="s">
         <v>480</v>
       </c>
       <c r="T72" s="9" t="s">
@@ -40988,7 +41003,7 @@
         <v>303</v>
       </c>
       <c r="AA72" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="AB72" t="s">
         <v>472</v>
@@ -41009,7 +41024,7 @@
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G73" s="26" t="s">
         <v>200</v>
@@ -41040,10 +41055,10 @@
       <c r="Q73" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R73" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S73" s="9" t="s">
+      <c r="R73" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S73" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T73" s="9" t="s">
@@ -41068,7 +41083,7 @@
         <v>348</v>
       </c>
       <c r="AA73" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB73" t="s">
         <v>301</v>
@@ -41090,7 +41105,7 @@
       </c>
       <c r="E74"/>
       <c r="F74" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="G74" t="e">
         <v>#N/A</v>
@@ -41122,10 +41137,10 @@
       <c r="Q74" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R74" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S74" s="9" t="s">
+      <c r="R74" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S74" s="5" t="s">
         <v>261</v>
       </c>
       <c r="T74" s="9" t="s">
@@ -41147,10 +41162,10 @@
         <v>1997</v>
       </c>
       <c r="Z74" t="s">
+        <v>756</v>
+      </c>
+      <c r="AA74" t="s">
         <v>757</v>
-      </c>
-      <c r="AA74" t="s">
-        <v>758</v>
       </c>
       <c r="AB74" t="s">
         <v>301</v>
@@ -41172,7 +41187,7 @@
       </c>
       <c r="E75"/>
       <c r="F75" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G75" t="s">
         <v>198</v>
@@ -41204,10 +41219,10 @@
       <c r="Q75" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R75" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S75" s="11" t="s">
+      <c r="R75" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S75" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T75" s="11" t="s">
@@ -41232,7 +41247,7 @@
         <v>348</v>
       </c>
       <c r="AA75" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB75" t="s">
         <v>301</v>
@@ -41254,7 +41269,7 @@
       </c>
       <c r="E76"/>
       <c r="F76" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G76" t="s">
         <v>198</v>
@@ -41286,10 +41301,10 @@
       <c r="Q76" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R76" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S76" s="11" t="s">
+      <c r="R76" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S76" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T76" s="11" t="s">
@@ -41314,7 +41329,7 @@
         <v>348</v>
       </c>
       <c r="AA76" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB76" t="s">
         <v>301</v>
@@ -41335,7 +41350,7 @@
         <v>177</v>
       </c>
       <c r="F77" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G77" s="24" t="s">
         <v>200</v>
@@ -41344,7 +41359,7 @@
         <v>192</v>
       </c>
       <c r="I77" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="J77" t="s">
         <v>177</v>
@@ -41370,10 +41385,10 @@
       <c r="Q77" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R77" s="9" t="s">
+      <c r="R77" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S77" s="9" t="s">
+      <c r="S77" s="5" t="s">
         <v>484</v>
       </c>
       <c r="T77" s="9" t="s">
@@ -41398,7 +41413,7 @@
         <v>481</v>
       </c>
       <c r="AA77" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="AB77" t="s">
         <v>482</v>
@@ -41421,7 +41436,7 @@
         <v>177</v>
       </c>
       <c r="F78" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G78" t="s">
         <v>198</v>
@@ -41436,7 +41451,7 @@
         <v>177</v>
       </c>
       <c r="K78" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="L78" s="30" t="s">
         <v>485</v>
@@ -41456,10 +41471,10 @@
       <c r="Q78" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R78" s="9" t="s">
+      <c r="R78" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="S78" s="9" t="s">
+      <c r="S78" s="5" t="s">
         <v>489</v>
       </c>
       <c r="T78" s="9" t="s">
@@ -41475,7 +41490,7 @@
         <v>301</v>
       </c>
       <c r="X78" s="9" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="Y78" s="4">
         <v>2014</v>
@@ -41484,7 +41499,7 @@
         <v>486</v>
       </c>
       <c r="AA78" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="AB78" t="s">
         <v>487</v>
@@ -41501,7 +41516,7 @@
         <v>177</v>
       </c>
       <c r="K79" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="L79" s="9" t="s">
         <v>490</v>
@@ -41521,10 +41536,10 @@
       <c r="Q79" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R79" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S79" s="9" t="s">
+      <c r="R79" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S79" s="5" t="s">
         <v>492</v>
       </c>
       <c r="T79" s="9" t="s">
@@ -41558,7 +41573,7 @@
         <v>177</v>
       </c>
       <c r="F80" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G80" s="7" t="s">
         <v>192</v>
@@ -41593,10 +41608,10 @@
       <c r="Q80" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R80" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S80" s="9" t="s">
+      <c r="R80" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S80" s="5" t="s">
         <v>497</v>
       </c>
       <c r="T80" s="9" t="s">
@@ -41621,7 +41636,7 @@
         <v>493</v>
       </c>
       <c r="AA80" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="AB80" t="s">
         <v>494</v>
@@ -41658,10 +41673,10 @@
       <c r="Q81" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R81" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S81" s="9" t="s">
+      <c r="R81" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S81" s="39" t="s">
         <v>267</v>
       </c>
       <c r="T81" s="9" t="s">
@@ -41693,7 +41708,7 @@
       </c>
       <c r="D82" s="9"/>
       <c r="F82" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G82" t="s">
         <v>198</v>
@@ -41724,10 +41739,10 @@
       <c r="Q82" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R82" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S82" s="11" t="s">
+      <c r="R82" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S82" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T82" s="11" t="s">
@@ -41752,26 +41767,26 @@
         <v>348</v>
       </c>
       <c r="AA82" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AD82" s="9"/>
     </row>
     <row r="83" spans="1:30">
       <c r="A83" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C83" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="D83" s="17" t="s">
         <v>699</v>
-      </c>
-      <c r="D83" s="17" t="s">
-        <v>700</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G83" s="2" t="e">
         <v>#N/A</v>
@@ -41786,10 +41801,10 @@
         <v>177</v>
       </c>
       <c r="K83" s="12" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="L83" s="28" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="M83" s="31" t="s">
         <v>269</v>
@@ -41806,11 +41821,11 @@
       <c r="Q83" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R83" s="12" t="s">
+      <c r="R83" s="38" t="s">
+        <v>700</v>
+      </c>
+      <c r="S83" s="35" t="s">
         <v>701</v>
-      </c>
-      <c r="S83" s="12" t="s">
-        <v>702</v>
       </c>
       <c r="T83" s="12" t="s">
         <v>203</v>
@@ -41831,13 +41846,13 @@
         <v>2018</v>
       </c>
       <c r="Z83" t="s">
+        <v>761</v>
+      </c>
+      <c r="AA83" t="s">
         <v>762</v>
       </c>
-      <c r="AA83" t="s">
-        <v>763</v>
-      </c>
       <c r="AB83" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="AC83" s="9">
         <v>2</v>
@@ -41870,15 +41885,15 @@
         <v>0</v>
       </c>
       <c r="P84" s="12" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="Q84" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R84" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S84" s="11" t="s">
+      <c r="R84" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S84" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T84" s="11" t="s">
@@ -41914,7 +41929,7 @@
         <v>268</v>
       </c>
       <c r="F85" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G85" s="24" t="s">
         <v>192</v>
@@ -41944,10 +41959,10 @@
       <c r="Q85" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R85" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S85" s="11" t="s">
+      <c r="R85" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S85" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T85" s="11" t="s">
@@ -41972,7 +41987,7 @@
         <v>348</v>
       </c>
       <c r="AA85" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB85" t="s">
         <v>301</v>
@@ -41994,7 +42009,7 @@
       </c>
       <c r="D86" s="9"/>
       <c r="F86" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G86" t="s">
         <v>198</v>
@@ -42025,10 +42040,10 @@
       <c r="Q86" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R86" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S86" s="11" t="s">
+      <c r="R86" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S86" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T86" s="11" t="s">
@@ -42053,7 +42068,7 @@
         <v>348</v>
       </c>
       <c r="AA86" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB86" t="s">
         <v>301</v>
@@ -42073,10 +42088,10 @@
         <v>177</v>
       </c>
       <c r="E87" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F87" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G87" s="24" t="s">
         <v>200</v>
@@ -42109,10 +42124,10 @@
       <c r="Q87" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R87" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S87" s="9" t="s">
+      <c r="R87" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S87" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T87" s="9" t="s">
@@ -42137,7 +42152,7 @@
         <v>500</v>
       </c>
       <c r="AA87" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="AB87" t="s">
         <v>501</v>
@@ -42172,10 +42187,10 @@
       <c r="Q88" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R88" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S88" s="9" t="s">
+      <c r="R88" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S88" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T88" s="9" t="s">
@@ -42213,15 +42228,15 @@
         <v>1</v>
       </c>
       <c r="P89" s="9" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="Q89" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R89" s="9" t="s">
+      <c r="R89" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S89" s="9" t="s">
+      <c r="S89" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T89" s="9" t="s">
@@ -42252,7 +42267,7 @@
         <v>177</v>
       </c>
       <c r="F90" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G90" t="e">
         <v>#N/A</v>
@@ -42287,10 +42302,10 @@
       <c r="Q90" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R90" s="9" t="s">
+      <c r="R90" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S90" s="9" t="s">
+      <c r="S90" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T90" s="9" t="s">
@@ -42315,7 +42330,7 @@
         <v>502</v>
       </c>
       <c r="AA90" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="AB90" t="s">
         <v>503</v>
@@ -42336,10 +42351,10 @@
       </c>
       <c r="D91" s="17"/>
       <c r="E91" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="F91" s="1" t="s">
         <v>676</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>677</v>
       </c>
       <c r="G91" s="1" t="e">
         <v>#N/A</v>
@@ -42377,7 +42392,7 @@
         <v>515</v>
       </c>
       <c r="AA91" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AB91" t="s">
         <v>516</v>
@@ -42416,10 +42431,10 @@
       <c r="Q92" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R92" s="9" t="s">
+      <c r="R92" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S92" s="9" t="s">
+      <c r="S92" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T92" s="9" t="s">
@@ -42449,27 +42464,27 @@
       <c r="I93" s="1"/>
       <c r="K93" s="13"/>
       <c r="L93" s="9" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="M93" s="10" t="s">
+        <v>708</v>
+      </c>
+      <c r="N93" s="9" t="s">
         <v>709</v>
-      </c>
-      <c r="N93" s="9" t="s">
-        <v>710</v>
       </c>
       <c r="O93" s="9">
         <v>0</v>
       </c>
       <c r="P93" s="9" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="Q93" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R93" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S93" s="9" t="s">
+      <c r="R93" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S93" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T93" s="9" t="s">
@@ -42504,7 +42519,7 @@
       </c>
       <c r="E94"/>
       <c r="F94" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G94" t="s">
         <v>198</v>
@@ -42539,10 +42554,10 @@
       <c r="Q94" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R94" s="9" t="s">
+      <c r="R94" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S94" s="9" t="s">
+      <c r="S94" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T94" s="9" t="s">
@@ -42567,7 +42582,7 @@
         <v>518</v>
       </c>
       <c r="AA94" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="AB94" t="s">
         <v>519</v>
@@ -42608,10 +42623,10 @@
       <c r="Q95" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R95" s="9" t="s">
+      <c r="R95" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S95" s="9" t="s">
+      <c r="S95" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T95" s="9" t="s">
@@ -42642,10 +42657,10 @@
         <v>177</v>
       </c>
       <c r="F96" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G96" s="17" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="H96" t="e">
         <v>#N/A</v>
@@ -42677,10 +42692,10 @@
       <c r="Q96" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R96" s="9" t="s">
+      <c r="R96" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S96" s="9" t="s">
+      <c r="S96" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T96" s="9" t="s">
@@ -42705,7 +42720,7 @@
         <v>520</v>
       </c>
       <c r="AA96" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="AB96" t="s">
         <v>521</v>
@@ -42742,10 +42757,10 @@
       <c r="Q97" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R97" s="9" t="s">
+      <c r="R97" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S97" s="9" t="s">
+      <c r="S97" s="5" t="s">
         <v>203</v>
       </c>
       <c r="T97" s="9" t="s">
@@ -42768,7 +42783,7 @@
         <v>348</v>
       </c>
       <c r="AA97" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB97" t="s">
         <v>301</v>
@@ -42791,7 +42806,7 @@
         <v>268</v>
       </c>
       <c r="F98" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G98" t="s">
         <v>198</v>
@@ -42823,10 +42838,10 @@
       <c r="Q98" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R98" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S98" s="11" t="s">
+      <c r="R98" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S98" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T98" s="11" t="s">
@@ -42860,10 +42875,10 @@
       </c>
       <c r="D99" s="9"/>
       <c r="E99" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F99" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G99" s="24" t="s">
         <v>192</v>
@@ -42892,10 +42907,10 @@
       <c r="Q99" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R99" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S99" s="11" t="s">
+      <c r="R99" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S99" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T99" s="11" t="s">
@@ -42920,7 +42935,7 @@
         <v>348</v>
       </c>
       <c r="AA99" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB99" t="s">
         <v>301</v>
@@ -42947,10 +42962,10 @@
       <c r="Q100" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R100" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S100" s="11" t="s">
+      <c r="R100" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S100" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T100" s="11" t="s">
@@ -43010,10 +43025,10 @@
       <c r="Q101" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R101" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S101" s="11" t="s">
+      <c r="R101" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S101" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T101" s="11" t="s">
@@ -43038,7 +43053,7 @@
         <v>348</v>
       </c>
       <c r="AA101" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB101" t="s">
         <v>301</v>
@@ -43087,10 +43102,10 @@
       <c r="Q102" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R102" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S102" s="11" t="s">
+      <c r="R102" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S102" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T102" s="11" t="s">
@@ -43115,7 +43130,7 @@
         <v>348</v>
       </c>
       <c r="AA102" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB102" t="s">
         <v>301</v>
@@ -43135,7 +43150,7 @@
         <v>177</v>
       </c>
       <c r="F103" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G103" s="17" t="s">
         <v>192</v>
@@ -43164,10 +43179,10 @@
       <c r="Q103" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R103" s="11" t="s">
+      <c r="R103" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="S103" s="11" t="s">
+      <c r="S103" s="34" t="s">
         <v>203</v>
       </c>
       <c r="T103" s="11" t="s">
@@ -43192,7 +43207,7 @@
         <v>303</v>
       </c>
       <c r="AA103" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="AB103" t="s">
         <v>522</v>
@@ -43212,7 +43227,7 @@
         <v>177</v>
       </c>
       <c r="F104" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G104" t="s">
         <v>198</v>
@@ -43241,10 +43256,10 @@
       <c r="Q104" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R104" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S104" s="11" t="s">
+      <c r="R104" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S104" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T104" s="11" t="s">
@@ -43266,10 +43281,10 @@
         <v>2001</v>
       </c>
       <c r="Z104" t="s">
+        <v>769</v>
+      </c>
+      <c r="AA104" t="s">
         <v>770</v>
-      </c>
-      <c r="AA104" t="s">
-        <v>771</v>
       </c>
       <c r="AB104" t="s">
         <v>301</v>
@@ -43280,7 +43295,7 @@
     </row>
     <row r="105" spans="1:30">
       <c r="F105" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="M105" s="14" t="s">
         <v>283</v>
@@ -43297,10 +43312,10 @@
       <c r="Q105" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R105" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S105" s="11" t="s">
+      <c r="R105" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S105" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T105" s="11" t="s">
@@ -43334,7 +43349,7 @@
         <v>177</v>
       </c>
       <c r="F106" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="G106" s="17" t="s">
         <v>192</v>
@@ -43363,10 +43378,10 @@
       <c r="Q106" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R106" s="11" t="s">
+      <c r="R106" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="S106" s="11" t="s">
+      <c r="S106" s="34" t="s">
         <v>203</v>
       </c>
       <c r="T106" s="11" t="s">
@@ -43391,7 +43406,7 @@
         <v>523</v>
       </c>
       <c r="AA106" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="AB106" t="s">
         <v>524</v>
@@ -43420,10 +43435,10 @@
       <c r="Q107" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R107" s="11" t="s">
+      <c r="R107" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="S107" s="11" t="s">
+      <c r="S107" s="34" t="s">
         <v>203</v>
       </c>
       <c r="T107" s="11" t="s">
@@ -43455,7 +43470,7 @@
         <v>177</v>
       </c>
       <c r="F108" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G108" t="e">
         <v>#N/A</v>
@@ -43484,10 +43499,10 @@
       <c r="Q108" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R108" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S108" s="11" t="s">
+      <c r="R108" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S108" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T108" s="11" t="s">
@@ -43512,7 +43527,7 @@
         <v>348</v>
       </c>
       <c r="AA108" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB108" t="s">
         <v>301</v>
@@ -43532,7 +43547,7 @@
         <v>177</v>
       </c>
       <c r="F109" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="G109" t="s">
         <v>198</v>
@@ -43561,10 +43576,10 @@
       <c r="Q109" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R109" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S109" s="11" t="s">
+      <c r="R109" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S109" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T109" s="11" t="s">
@@ -43589,7 +43604,7 @@
         <v>348</v>
       </c>
       <c r="AA109" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB109" t="s">
         <v>301</v>
@@ -43609,7 +43624,7 @@
         <v>177</v>
       </c>
       <c r="F110" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G110" s="17" t="s">
         <v>192</v>
@@ -43641,10 +43656,10 @@
       <c r="Q110" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R110" s="9" t="s">
+      <c r="R110" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S110" s="11" t="s">
+      <c r="S110" s="34" t="s">
         <v>203</v>
       </c>
       <c r="T110" s="11" t="s">
@@ -43669,7 +43684,7 @@
         <v>404</v>
       </c>
       <c r="AA110" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="AB110" t="s">
         <v>525</v>
@@ -43689,7 +43704,7 @@
         <v>177</v>
       </c>
       <c r="F111" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G111" s="7" t="s">
         <v>192</v>
@@ -43718,10 +43733,10 @@
       <c r="Q111" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R111" s="9" t="s">
+      <c r="R111" s="17" t="s">
         <v>556</v>
       </c>
-      <c r="S111" s="11" t="s">
+      <c r="S111" s="34" t="s">
         <v>555</v>
       </c>
       <c r="T111" s="11" t="s">
@@ -43746,7 +43761,7 @@
         <v>526</v>
       </c>
       <c r="AA111" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="AB111" t="s">
         <v>527</v>
@@ -43766,19 +43781,19 @@
         <v>177</v>
       </c>
       <c r="D112" s="17" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E112" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F112" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G112" s="7" t="s">
         <v>200</v>
       </c>
       <c r="H112" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I112" t="e">
         <v>#N/A</v>
@@ -43804,10 +43819,10 @@
       <c r="Q112" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R112" s="9" t="s">
+      <c r="R112" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="S112" s="11" t="s">
+      <c r="S112" s="34" t="s">
         <v>203</v>
       </c>
       <c r="T112" s="11" t="s">
@@ -43832,10 +43847,10 @@
         <v>528</v>
       </c>
       <c r="AA112" t="s">
+        <v>774</v>
+      </c>
+      <c r="AB112" t="s">
         <v>775</v>
-      </c>
-      <c r="AB112" t="s">
-        <v>776</v>
       </c>
       <c r="AC112">
         <v>10</v>
@@ -43866,10 +43881,10 @@
       <c r="Q113" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R113" s="9" t="s">
+      <c r="R113" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S113" s="11" t="s">
+      <c r="S113" s="34" t="s">
         <v>203</v>
       </c>
       <c r="T113" s="11" t="s">
@@ -43909,10 +43924,10 @@
       <c r="Q114" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="R114" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="S114" s="9" t="s">
+      <c r="R114" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="S114" s="5" t="s">
         <v>301</v>
       </c>
       <c r="T114" s="9" t="s">
@@ -43943,7 +43958,7 @@
         <v>177</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G115" s="24" t="s">
         <v>192</v>
@@ -43972,10 +43987,10 @@
       <c r="Q115" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R115" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S115" s="11" t="s">
+      <c r="R115" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S115" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T115" s="11" t="s">
@@ -44000,7 +44015,7 @@
         <v>348</v>
       </c>
       <c r="AA115" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="AB115" t="s">
         <v>301</v>
@@ -44021,7 +44036,7 @@
       </c>
       <c r="E116" s="1"/>
       <c r="F116" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G116" s="1" t="s">
         <v>198</v>
@@ -44053,10 +44068,10 @@
       <c r="Q116" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R116" s="9" t="s">
+      <c r="R116" s="17" t="s">
         <v>567</v>
       </c>
-      <c r="S116" s="11" t="s">
+      <c r="S116" s="34" t="s">
         <v>203</v>
       </c>
       <c r="T116" s="11" t="s">
@@ -44081,7 +44096,7 @@
         <v>305</v>
       </c>
       <c r="AA116" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="AB116" t="s">
         <v>529</v>
@@ -44101,7 +44116,7 @@
         <v>177</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G117" t="s">
         <v>198</v>
@@ -44130,10 +44145,10 @@
       <c r="Q117" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R117" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S117" s="11" t="s">
+      <c r="R117" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S117" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T117" s="11" t="s">
@@ -44158,7 +44173,7 @@
         <v>348</v>
       </c>
       <c r="AA117" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB117" t="s">
         <v>301</v>
@@ -44179,7 +44194,7 @@
       </c>
       <c r="E118" s="1"/>
       <c r="F118" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G118" s="1" t="e">
         <v>#N/A</v>
@@ -44211,10 +44226,10 @@
       <c r="Q118" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R118" s="9" t="s">
+      <c r="R118" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S118" s="9" t="s">
+      <c r="S118" s="5" t="s">
         <v>569</v>
       </c>
       <c r="T118" s="11" t="s">
@@ -44239,7 +44254,7 @@
         <v>404</v>
       </c>
       <c r="AA118" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="AB118" t="s">
         <v>530</v>
@@ -44262,7 +44277,7 @@
         <v>177</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G119" t="s">
         <v>198</v>
@@ -44294,10 +44309,10 @@
       <c r="Q119" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R119" s="9" t="s">
+      <c r="R119" s="17" t="s">
         <v>572</v>
       </c>
-      <c r="S119" s="11" t="s">
+      <c r="S119" s="34" t="s">
         <v>571</v>
       </c>
       <c r="T119" s="11" t="s">
@@ -44322,7 +44337,7 @@
         <v>430</v>
       </c>
       <c r="AA119" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="AB119" t="s">
         <v>531</v>
@@ -44346,7 +44361,7 @@
       </c>
       <c r="E120" s="1"/>
       <c r="F120" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G120" s="25" t="s">
         <v>192</v>
@@ -44378,11 +44393,11 @@
       <c r="Q120" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R120" s="9" t="s">
+      <c r="R120" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="S120" s="11" t="s">
-        <v>575</v>
+      <c r="S120" s="34" t="s">
+        <v>783</v>
       </c>
       <c r="T120" s="11" t="s">
         <v>203</v>
@@ -44394,7 +44409,7 @@
         <v>203</v>
       </c>
       <c r="W120" s="9" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="X120" s="11" t="s">
         <v>203</v>
@@ -44406,7 +44421,7 @@
         <v>367</v>
       </c>
       <c r="AA120" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="AB120" t="s">
         <v>532</v>
@@ -44426,7 +44441,7 @@
         <v>177</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="G121" t="s">
         <v>198</v>
@@ -44452,10 +44467,10 @@
       <c r="Q121" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="R121" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="S121" s="11" t="s">
+      <c r="R121" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="S121" s="34" t="s">
         <v>301</v>
       </c>
       <c r="T121" s="11" t="s">
@@ -44480,7 +44495,7 @@
         <v>348</v>
       </c>
       <c r="AA121" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="AB121" t="s">
         <v>301</v>
@@ -44497,7 +44512,7 @@
         <v>176</v>
       </c>
       <c r="C122" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D122" t="s">
         <v>177</v>
@@ -44516,7 +44531,7 @@
         <v>534</v>
       </c>
       <c r="L122" s="9" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="M122" s="10" t="s">
         <v>295</v>
@@ -44533,11 +44548,11 @@
       <c r="Q122" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="R122" s="9" t="s">
+      <c r="R122" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="S122" t="s">
-        <v>578</v>
+      <c r="S122" s="5" t="s">
+        <v>577</v>
       </c>
       <c r="T122" s="11" t="s">
         <v>190</v>
@@ -44561,7 +44576,7 @@
         <v>533</v>
       </c>
       <c r="AA122" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="AB122" t="s">
         <v>534</v>

</xml_diff>